<commit_message>
Update for Allure reports and TestEnvironment base class
</commit_message>
<xml_diff>
--- a/src/test/resources/bluesource/dataProviders/TestAddNewDept.xlsx
+++ b/src/test/resources/bluesource/dataProviders/TestAddNewDept.xlsx
@@ -1,13 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\git\Java-Automation-Framework\src\test\resources\bluesource\dataProviders\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="18195" windowHeight="6975"/>
+    <workbookView xWindow="0" yWindow="140" windowWidth="18200" windowHeight="6980"/>
   </bookViews>
   <sheets>
-    <sheet name="TestAddNewTitle" sheetId="1" r:id="rId1"/>
+    <sheet name="TestAddNewDept" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -37,8 +42,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -565,6 +570,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -611,7 +624,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -643,9 +656,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -677,6 +691,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -852,16 +867,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -872,7 +887,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Adding test cases for feature Login
</commit_message>
<xml_diff>
--- a/src/test/resources/bluesource/dataProviders/TestAddNewDept.xlsx
+++ b/src/test/resources/bluesource/dataProviders/TestAddNewDept.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>TestScenario</t>
   </si>
@@ -30,13 +30,49 @@
     <t>COMPANY_ADMIN</t>
   </si>
   <si>
-    <t>Test1234</t>
-  </si>
-  <si>
     <t>NewDepartment</t>
   </si>
   <si>
-    <t>Add a new department</t>
+    <t>DEPARTMENT_ADMIN</t>
+  </si>
+  <si>
+    <t>DEPARTMENT_HEAD</t>
+  </si>
+  <si>
+    <t>UPPER_MANAGEMENT</t>
+  </si>
+  <si>
+    <t>MANAGEMENT</t>
+  </si>
+  <si>
+    <t>Add a new department as Company Admin</t>
+  </si>
+  <si>
+    <t>Test_COMPANY_ADMIN_department</t>
+  </si>
+  <si>
+    <t>Add a new department as Department Admin</t>
+  </si>
+  <si>
+    <t>Test_DEPARTMENT_ADMIN_department</t>
+  </si>
+  <si>
+    <t>Add a new department as Department Head</t>
+  </si>
+  <si>
+    <t>Test_DEPARTMENT_HEAD_department</t>
+  </si>
+  <si>
+    <t>Add a new department as Upper Management</t>
+  </si>
+  <si>
+    <t>Test_UPPER_MANAGEMENT_department</t>
+  </si>
+  <si>
+    <t>Add a new department as Management</t>
+  </si>
+  <si>
+    <t>Test_MANAGEMENT_department</t>
   </si>
 </sst>
 </file>
@@ -868,13 +904,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="33.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -884,18 +925,62 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>